<commit_message>
fix previous period hold-over subscription's first action being manual unsubscriptions not being counted
</commit_message>
<xml_diff>
--- a/backend/checkpoints/base-ETH-TEL-14.xlsx
+++ b/backend/checkpoints/base-ETH-TEL-14.xlsx
@@ -7151,7 +7151,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7184,7 +7184,7 @@
         <v>0.8</v>
       </c>
       <c r="D2" t="str">
-        <v>12.15</v>
+        <v>6.89</v>
       </c>
       <c r="E2" t="str">
         <v>160</v>
@@ -7201,7 +7201,7 @@
         <v>1738.04</v>
       </c>
       <c r="D3" t="str">
-        <v>26415.28</v>
+        <v>14969.18</v>
       </c>
       <c r="E3" t="str">
         <v>347608</v>
@@ -7218,7 +7218,7 @@
         <v>183.93</v>
       </c>
       <c r="D4" t="str">
-        <v>2514.1</v>
+        <v>1424.7</v>
       </c>
       <c r="E4" t="str">
         <v>33084</v>
@@ -7252,7 +7252,7 @@
         <v>140.84</v>
       </c>
       <c r="D6" t="str">
-        <v>2409.69</v>
+        <v>1365.54</v>
       </c>
       <c r="E6" t="str">
         <v>31710</v>
@@ -7260,81 +7260,81 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>0x4651B2E464e94c730725F3D5B2737418E2e5fd32</v>
+        <v>0x8F1c51E98Af7C7dbB24654ACB05781E0e96e008F</v>
       </c>
       <c r="B7" t="str">
-        <v>0.019648622723011631</v>
+        <v>0.082142650014355746</v>
       </c>
       <c r="C7" t="str">
-        <v>9500.17</v>
+        <v>42455.63</v>
       </c>
       <c r="D7" t="str">
-        <v>144386.61</v>
+        <v>353860.12</v>
       </c>
       <c r="E7" t="str">
-        <v>1900034</v>
+        <v>8217188</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>0xdcE6F2ccaf54de860a5f80DB7503154957d216D5</v>
+        <v>0x4651B2E464e94c730725F3D5B2737418E2e5fd32</v>
       </c>
       <c r="B8" t="str">
-        <v>0.011259589849224022</v>
+        <v>0.019648622723011631</v>
       </c>
       <c r="C8" t="str">
-        <v>5248.44</v>
+        <v>9500.17</v>
       </c>
       <c r="D8" t="str">
-        <v>0</v>
+        <v>81821.94</v>
       </c>
       <c r="E8" t="str">
-        <v>0</v>
+        <v>1900034</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>0xBa44825f3215A71b34a702A70373afF8d4A52390</v>
+        <v>0x0380ad3322Df94334C2f30CEE24D3086FC6F3445</v>
       </c>
       <c r="B9" t="str">
-        <v>0.009905592850166421</v>
+        <v>0.00381512308505338</v>
       </c>
       <c r="C9" t="str">
-        <v>5029</v>
+        <v>1268.64</v>
       </c>
       <c r="D9" t="str">
-        <v>74611.43</v>
+        <v>0</v>
       </c>
       <c r="E9" t="str">
-        <v>981838</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>0xc38eDb1B53c7c034867BdE801e24826687F24466</v>
+        <v>0x2fe6f7c52EccC8Fea03289EC10213033a7c364b7</v>
       </c>
       <c r="B10" t="str">
-        <v>0.008026972749126571</v>
+        <v>0.000276182821902365</v>
       </c>
       <c r="C10" t="str">
-        <v>4457.34</v>
+        <v>61.39</v>
       </c>
       <c r="D10" t="str">
-        <v>12643.17</v>
+        <v>0</v>
       </c>
       <c r="E10" t="str">
-        <v>166376</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>0xabF76381Ab5538598AA4cd77d01De16c3F48a54A</v>
+        <v>0xdcE6F2ccaf54de860a5f80DB7503154957d216D5</v>
       </c>
       <c r="B11" t="str">
-        <v>0.003697156090803694</v>
+        <v>0.011746297729462631</v>
       </c>
       <c r="C11" t="str">
-        <v>1259.12</v>
+        <v>5386.43</v>
       </c>
       <c r="D11" t="str">
         <v>0</v>
@@ -7345,160 +7345,245 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>0x2fe6f7c52EccC8Fea03289EC10213033a7c364b7</v>
+        <v>0xBa44825f3215A71b34a702A70373afF8d4A52390</v>
       </c>
       <c r="B12" t="str">
-        <v>0</v>
+        <v>0.009905592850166421</v>
       </c>
       <c r="C12" t="str">
-        <v>0</v>
+        <v>5029</v>
       </c>
       <c r="D12" t="str">
-        <v>0</v>
+        <v>42281.29</v>
       </c>
       <c r="E12" t="str">
-        <v>0</v>
+        <v>981838</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>0x87029960cb6d1011289d35bC8944d37B88C46B72</v>
+        <v>0xa614A83132a2e7368aDa71dA9331817c33706770</v>
       </c>
       <c r="B13" t="str">
-        <v>0.001735955596785356</v>
+        <v>0</v>
       </c>
       <c r="C13" t="str">
-        <v>764.19</v>
+        <v>0</v>
       </c>
       <c r="D13" t="str">
-        <v>8776.34</v>
+        <v>0</v>
       </c>
       <c r="E13" t="str">
-        <v>115491</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>0x92119de4787cb947A4A93FEEC7c19C3AFe1b5729</v>
+        <v>0xc38eDb1B53c7c034867BdE801e24826687F24466</v>
       </c>
       <c r="B14" t="str">
-        <v>0.123174058999187785</v>
+        <v>0.008026972749126571</v>
       </c>
       <c r="C14" t="str">
-        <v>60862.03</v>
+        <v>4457.34</v>
       </c>
       <c r="D14" t="str">
-        <v>0</v>
+        <v>7164.71</v>
       </c>
       <c r="E14" t="str">
-        <v>0</v>
+        <v>166376</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>0x5196E6ff6b95536874ba6405c11f465e026099e0</v>
+        <v>0xabF76381Ab5538598AA4cd77d01De16c3F48a54A</v>
       </c>
       <c r="B15" t="str">
-        <v>0.000550477048328321</v>
+        <v>0.003697156090803694</v>
       </c>
       <c r="C15" t="str">
-        <v>227.09</v>
+        <v>1259.12</v>
       </c>
       <c r="D15" t="str">
-        <v>3748.2</v>
+        <v>0</v>
       </c>
       <c r="E15" t="str">
-        <v>49324</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>0xCDA0c8a5f22565ae0efB889E5dBb6CE60498d0b4</v>
+        <v>0xf51435DD16E9a346f016A0a9123A7A87D80b28AA</v>
       </c>
       <c r="B16" t="str">
-        <v>0.01020271109981372</v>
+        <v>0.003600962835922976</v>
       </c>
       <c r="C16" t="str">
-        <v>4286.15</v>
+        <v>1922.75</v>
       </c>
       <c r="D16" t="str">
-        <v>0</v>
+        <v>15777.65</v>
       </c>
       <c r="E16" t="str">
-        <v>0</v>
+        <v>366382</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>0xe3B1ebcD19c28459aD75B44C13095cA93E53cbB0</v>
+        <v>0xf5DFA78573d859Ba64522B44FF0F7f970cFc5D78</v>
       </c>
       <c r="B17" t="str">
-        <v>0.00092088557386215</v>
+        <v>0.011698625575774027</v>
       </c>
       <c r="C17" t="str">
-        <v>387.47</v>
+        <v>4055.78</v>
       </c>
       <c r="D17" t="str">
-        <v>6327.97</v>
+        <v>0</v>
       </c>
       <c r="E17" t="str">
-        <v>83272</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>0xf6786b4edFa78d8d5cbfB93A97fF260e873152Be</v>
+        <v>0x5196E6ff6b95536874ba6405c11f465e026099e0</v>
       </c>
       <c r="B18" t="str">
-        <v>0.023721435439256031</v>
+        <v>0.00118886197213139</v>
       </c>
       <c r="C18" t="str">
-        <v>10008.11</v>
+        <v>574.7</v>
       </c>
       <c r="D18" t="str">
-        <v>163210.95</v>
+        <v>4950.18</v>
       </c>
       <c r="E18" t="str">
-        <v>2147750</v>
+        <v>114951</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>0x8F1c51E98Af7C7dbB24654ACB05781E0e96e008F</v>
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
       </c>
       <c r="B19" t="str">
-        <v>0.028370995005692445</v>
+        <v>0</v>
       </c>
       <c r="C19" t="str">
-        <v>12887.65</v>
+        <v>0</v>
       </c>
       <c r="D19" t="str">
-        <v>202176.55</v>
+        <v>0</v>
       </c>
       <c r="E19" t="str">
-        <v>2660512</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>0xf51435DD16E9a346f016A0a9123A7A87D80b28AA</v>
+        <v>0x87029960cb6d1011289d35bC8944d37B88C46B72</v>
       </c>
       <c r="B20" t="str">
-        <v>0.000132406609078396</v>
+        <v>0.001735955596785356</v>
       </c>
       <c r="C20" t="str">
-        <v>56.48</v>
+        <v>764.19</v>
       </c>
       <c r="D20" t="str">
-        <v>915.62</v>
+        <v>4973.43</v>
       </c>
       <c r="E20" t="str">
-        <v>12049</v>
+        <v>115491</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>0x3663b2EE275616bfA14e77c69dc02b79e6C580F0</v>
+      </c>
+      <c r="B21" t="str">
+        <v>0.005049157278053823</v>
+      </c>
+      <c r="C21" t="str">
+        <v>3010.46</v>
+      </c>
+      <c r="D21" t="str">
+        <v>23477.05</v>
+      </c>
+      <c r="E21" t="str">
+        <v>545174</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>0x92119de4787cb947A4A93FEEC7c19C3AFe1b5729</v>
+      </c>
+      <c r="B22" t="str">
+        <v>0.123174058999187785</v>
+      </c>
+      <c r="C22" t="str">
+        <v>60862.03</v>
+      </c>
+      <c r="D22" t="str">
+        <v>0</v>
+      </c>
+      <c r="E22" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>0xCDA0c8a5f22565ae0efB889E5dBb6CE60498d0b4</v>
+      </c>
+      <c r="B23" t="str">
+        <v>0.01020271109981372</v>
+      </c>
+      <c r="C23" t="str">
+        <v>4286.15</v>
+      </c>
+      <c r="D23" t="str">
+        <v>0</v>
+      </c>
+      <c r="E23" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>0xe3B1ebcD19c28459aD75B44C13095cA93E53cbB0</v>
+      </c>
+      <c r="B24" t="str">
+        <v>0.00092088557386215</v>
+      </c>
+      <c r="C24" t="str">
+        <v>387.47</v>
+      </c>
+      <c r="D24" t="str">
+        <v>3585.97</v>
+      </c>
+      <c r="E24" t="str">
+        <v>83272</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>0xf6786b4edFa78d8d5cbfB93A97fF260e873152Be</v>
+      </c>
+      <c r="B25" t="str">
+        <v>0.023721435439256031</v>
+      </c>
+      <c r="C25" t="str">
+        <v>10008.11</v>
+      </c>
+      <c r="D25" t="str">
+        <v>92489.43</v>
+      </c>
+      <c r="E25" t="str">
+        <v>2147750</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>